<commit_message>
Fixed Tranform Paramter format.
The transform parameters are now in YAML format.
</commit_message>
<xml_diff>
--- a/bmsapp/scripts/files/add_sensors_sample.xlsx
+++ b/bmsapp/scripts/files/add_sensors_sample.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -129,9 +129,6 @@
     <t>linear</t>
   </si>
   <si>
-    <t>id_val="chuvw_firing_rate_tot", slope=30000.0</t>
-  </si>
-  <si>
     <t>Building</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Function Parameters</t>
+  </si>
+  <si>
+    <t>id_val: chuvw_firing_rate_tot\nslope: 30000.0</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,31 +578,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>